<commit_message>
[ADD] Test excel file load system. But this is not good method. I will test another one.
</commit_message>
<xml_diff>
--- a/RPG_Game/StageData.xlsx
+++ b/RPG_Game/StageData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TeamSparta\PersonalProject\RPG_Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56CE6014-4C5C-40DB-98BB-DBBE1996696E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1A7ABB6-FB79-41FC-BD2C-E3DD8EBD4129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="2355" windowWidth="16020" windowHeight="12465" xr2:uid="{288195C0-BF66-4B03-812C-610F85EA7E9A}"/>
+    <workbookView xWindow="7650" yWindow="3135" windowWidth="16020" windowHeight="12465" xr2:uid="{288195C0-BF66-4B03-812C-610F85EA7E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,31 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>hi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hihi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hihihi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hihihihi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wow!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -394,12 +419,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916C3D32-73B2-4E29-A1B0-939B6863675E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>